<commit_message>
Removed some unncessary files
</commit_message>
<xml_diff>
--- a/civilization/src/main/resources/gamedata-faf-waw.xlsx
+++ b/civilization/src/main/resources/gamedata-faf-waw.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" firstSheet="3" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Civ" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="302">
   <si>
     <t>Civilization</t>
   </si>
@@ -1299,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,153 +1314,103 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
-        <f t="shared" ref="B2:B17" ca="1" si="0">RAND()</f>
-        <v>0.60069855456013388</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.49231347236485856</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.38943822040848974</v>
-      </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.42363999986852696</v>
-      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.79197981818287111</v>
-      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.29227930107171918</v>
-      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.60888227652421256</v>
-      </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.87399560507531382</v>
-      </c>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0747721651500619E-2</v>
-      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.57800754647887542</v>
-      </c>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.8799213021228115</v>
-      </c>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.77354823538087203</v>
-      </c>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.70805966978692125</v>
-      </c>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.3954170085873896</v>
-      </c>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.665055881658863E-2</v>
-      </c>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.95086290796803818</v>
-      </c>
+      <c r="B17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1473,7 +1423,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1485,189 +1435,127 @@
       <c r="A1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>201</v>
       </c>
-      <c r="B2" s="2">
-        <f t="shared" ref="B2:B21" ca="1" si="0">RAND()</f>
-        <v>0.68796878238863546</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>201</v>
       </c>
-      <c r="B3" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.15923914318622079</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>201</v>
       </c>
-      <c r="B4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.41181653413814068</v>
-      </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>203</v>
       </c>
-      <c r="B5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.29418445514235936</v>
-      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>205</v>
       </c>
-      <c r="B6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.18678059808466452</v>
-      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>205</v>
       </c>
-      <c r="B7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.36782788010437062</v>
-      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>206</v>
       </c>
-      <c r="B8" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.2292913915178153</v>
-      </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>206</v>
       </c>
-      <c r="B9" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.39414809061330558</v>
-      </c>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>206</v>
       </c>
-      <c r="B10" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.42000070209676366</v>
-      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>207</v>
       </c>
-      <c r="B11" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.95946832025742179</v>
-      </c>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>208</v>
       </c>
-      <c r="B12" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.19388725338073887</v>
-      </c>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>208</v>
       </c>
-      <c r="B13" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.87500794402093918</v>
-      </c>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>208</v>
       </c>
-      <c r="B14" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.84322559998991542</v>
-      </c>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>208</v>
       </c>
-      <c r="B15" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.82144145050683881</v>
-      </c>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>211</v>
       </c>
-      <c r="B16" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.10388152611292978</v>
-      </c>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>211</v>
       </c>
-      <c r="B17" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.70588300835006879</v>
-      </c>
+      <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>211</v>
       </c>
-      <c r="B18" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.4108819570102541</v>
-      </c>
+      <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>211</v>
       </c>
-      <c r="B19" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.15344532235503117</v>
-      </c>
+      <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>212</v>
       </c>
-      <c r="B20" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.65788457571613612</v>
-      </c>
+      <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>212</v>
       </c>
-      <c r="B21" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.85599693820337075</v>
-      </c>
+      <c r="B21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1679,7 +1567,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,324 +1580,217 @@
       <c r="A1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>201</v>
       </c>
-      <c r="B2" s="2">
-        <f t="shared" ref="B2:B36" ca="1" si="0">RAND()</f>
-        <v>0.23662129062660398</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>201</v>
       </c>
-      <c r="B3" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.17260182274390268</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>202</v>
       </c>
-      <c r="B4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.19900642557400405</v>
-      </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0787513624490153E-2</v>
-      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>204</v>
       </c>
-      <c r="B6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.12750658839323148</v>
-      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>204</v>
       </c>
-      <c r="B7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.87355170938924664</v>
-      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>204</v>
       </c>
-      <c r="B8" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.90081807479539155</v>
-      </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>204</v>
       </c>
-      <c r="B9" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.14982453259205886</v>
-      </c>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>204</v>
       </c>
-      <c r="B10" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.70847624624246774</v>
-      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>204</v>
       </c>
-      <c r="B11" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.13445817512139047</v>
-      </c>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>206</v>
       </c>
-      <c r="B12" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.9533500419537807</v>
-      </c>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.30175746796523539</v>
-      </c>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>206</v>
       </c>
-      <c r="B14" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.44734575359721218</v>
-      </c>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>209</v>
       </c>
-      <c r="B15" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.77655296834060561</v>
-      </c>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>210</v>
       </c>
-      <c r="B16" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.5447686839222976</v>
-      </c>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>210</v>
       </c>
-      <c r="B17" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.93940348956307285</v>
-      </c>
+      <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>210</v>
       </c>
-      <c r="B18" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.72033086858248407</v>
-      </c>
+      <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>210</v>
       </c>
-      <c r="B19" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.38936668394062146</v>
-      </c>
+      <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>210</v>
       </c>
-      <c r="B20" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.36154025484134444</v>
-      </c>
+      <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>210</v>
       </c>
-      <c r="B21" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.29252389568320447</v>
-      </c>
+      <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>208</v>
       </c>
-      <c r="B22" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.76883997288951345</v>
-      </c>
+      <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>208</v>
       </c>
-      <c r="B23" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.29470770174180727</v>
-      </c>
+      <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>208</v>
       </c>
-      <c r="B24" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.13542514235483927</v>
-      </c>
+      <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>208</v>
       </c>
-      <c r="B25" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.5976206152606417</v>
-      </c>
+      <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>208</v>
       </c>
-      <c r="B26" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.82902849911800891</v>
-      </c>
+      <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>208</v>
       </c>
-      <c r="B27" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.81346987364672763</v>
-      </c>
+      <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>213</v>
       </c>
-      <c r="B28" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.95620329969168061</v>
-      </c>
+      <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>211</v>
       </c>
-      <c r="B29" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.21937424567974761</v>
-      </c>
+      <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>214</v>
       </c>
-      <c r="B30" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.16262219987679494</v>
-      </c>
+      <c r="B30" s="2"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>214</v>
       </c>
-      <c r="B31" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.91633101630744751</v>
-      </c>
+      <c r="B31" s="2"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>214</v>
       </c>
-      <c r="B32" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.20115044327035536</v>
-      </c>
+      <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>214</v>
       </c>
-      <c r="B33" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.49967141783865821</v>
-      </c>
+      <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>214</v>
       </c>
-      <c r="B34" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.32339945694511407</v>
-      </c>
+      <c r="B34" s="2"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>214</v>
       </c>
-      <c r="B35" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.45194594966557144</v>
-      </c>
+      <c r="B35" s="2"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>214</v>
       </c>
-      <c r="B36" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.24219414071978052</v>
-      </c>
+      <c r="B36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2021,8 +1802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2048,9 +1829,7 @@
       <c r="D1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2065,10 +1844,7 @@
       <c r="D2" t="s">
         <v>220</v>
       </c>
-      <c r="E2" s="2">
-        <f t="shared" ref="E2:E10" ca="1" si="0">RAND()</f>
-        <v>0.1493827158775981</v>
-      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2080,10 +1856,7 @@
       <c r="C3">
         <v>15</v>
       </c>
-      <c r="E3" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.896987719998172E-2</v>
-      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2095,10 +1868,7 @@
       <c r="C4">
         <v>10</v>
       </c>
-      <c r="E4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.9194136976872892</v>
-      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2113,10 +1883,7 @@
       <c r="D5" t="s">
         <v>227</v>
       </c>
-      <c r="E5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.67633992155433931</v>
-      </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2131,10 +1898,7 @@
       <c r="D6" t="s">
         <v>230</v>
       </c>
-      <c r="E6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.92224956193318375</v>
-      </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2149,10 +1913,7 @@
       <c r="D7" t="s">
         <v>233</v>
       </c>
-      <c r="E7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.25466335208137547</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2167,10 +1928,7 @@
       <c r="D8" t="s">
         <v>236</v>
       </c>
-      <c r="E8" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.26705705646468902</v>
-      </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2185,10 +1943,7 @@
       <c r="D9" t="s">
         <v>239</v>
       </c>
-      <c r="E9" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.24032146590658898</v>
-      </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2203,10 +1958,7 @@
       <c r="D10" t="s">
         <v>242</v>
       </c>
-      <c r="E10" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.24446027017182359</v>
-      </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -2221,9 +1973,7 @@
       <c r="D12" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2238,10 +1988,7 @@
       <c r="D13" t="s">
         <v>246</v>
       </c>
-      <c r="E13" s="2">
-        <f t="shared" ref="E13:E21" ca="1" si="1">RAND()</f>
-        <v>0.86733231333862404</v>
-      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2253,10 +2000,7 @@
       <c r="C14">
         <v>15</v>
       </c>
-      <c r="E14" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.68361158694408231</v>
-      </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2271,10 +2015,7 @@
       <c r="D15" t="s">
         <v>251</v>
       </c>
-      <c r="E15" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.67226921973737508</v>
-      </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2289,10 +2030,7 @@
       <c r="D16" t="s">
         <v>254</v>
       </c>
-      <c r="E16" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.65467007444770098</v>
-      </c>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -2307,10 +2045,7 @@
       <c r="D17" t="s">
         <v>257</v>
       </c>
-      <c r="E17" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.74104798647560299</v>
-      </c>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -2325,10 +2060,7 @@
       <c r="D18" t="s">
         <v>260</v>
       </c>
-      <c r="E18" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.65553088455953767</v>
-      </c>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -2343,10 +2075,7 @@
       <c r="D19" t="s">
         <v>263</v>
       </c>
-      <c r="E19" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.15231386105928679</v>
-      </c>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2361,10 +2090,7 @@
       <c r="D20" t="s">
         <v>266</v>
       </c>
-      <c r="E20" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.51765505881482921</v>
-      </c>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -2379,10 +2105,7 @@
       <c r="D21" t="s">
         <v>269</v>
       </c>
-      <c r="E21" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.17336917556298481</v>
-      </c>
+      <c r="E21" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -2397,9 +2120,7 @@
       <c r="D23" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -2414,10 +2135,7 @@
       <c r="D24" t="s">
         <v>273</v>
       </c>
-      <c r="E24" s="2">
-        <f t="shared" ref="E24:E32" ca="1" si="2">RAND()</f>
-        <v>0.12751134369176309</v>
-      </c>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -2432,10 +2150,7 @@
       <c r="D25" t="s">
         <v>276</v>
       </c>
-      <c r="E25" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.3585290115345714</v>
-      </c>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -2450,10 +2165,7 @@
       <c r="D26" t="s">
         <v>279</v>
       </c>
-      <c r="E26" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.59331337044991672</v>
-      </c>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -2468,10 +2180,7 @@
       <c r="D27" t="s">
         <v>282</v>
       </c>
-      <c r="E27" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.39044062738456697</v>
-      </c>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -2483,10 +2192,7 @@
       <c r="C28">
         <v>25</v>
       </c>
-      <c r="E28" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.18052988834486861</v>
-      </c>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -2501,10 +2207,7 @@
       <c r="D29" t="s">
         <v>287</v>
       </c>
-      <c r="E29" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.7106948268703569</v>
-      </c>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -2519,10 +2222,7 @@
       <c r="D30" t="s">
         <v>290</v>
       </c>
-      <c r="E30" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.87488827694076876</v>
-      </c>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -2537,10 +2237,7 @@
       <c r="D31" t="s">
         <v>293</v>
       </c>
-      <c r="E31" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.71996808735373929</v>
-      </c>
+      <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -2552,10 +2249,7 @@
       <c r="C32">
         <v>20</v>
       </c>
-      <c r="E32" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.13558401973154333</v>
-      </c>
+      <c r="E32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2568,7 +2262,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2581,252 +2275,169 @@
       <c r="A1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <f t="shared" ref="B2:B28" ca="1" si="0">RAND()</f>
-        <v>0.66244742946357915</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.62863014366790848</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.15844890754294538</v>
-      </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.6217900218417286</v>
-      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.95314183893161331</v>
-      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.58312730946865099</v>
-      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.89707841950504386</v>
-      </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.13829080716948283</v>
-      </c>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.72048258074581994</v>
-      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.4728377356314546E-3</v>
-      </c>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.6146557449345194E-2</v>
-      </c>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.67848811838539114</v>
-      </c>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.86673161202940519</v>
-      </c>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.48071600642831769</v>
-      </c>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.85513868413938587</v>
-      </c>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.4525374194541687</v>
-      </c>
+      <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.36646498482218048</v>
-      </c>
+      <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.20717795325786281</v>
-      </c>
+      <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.45847374815458586</v>
-      </c>
+      <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.8432466346817424E-2</v>
-      </c>
+      <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.43109668027364778</v>
-      </c>
+      <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.66327380515617895</v>
-      </c>
+      <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>23</v>
       </c>
-      <c r="B24" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.29005578914040031</v>
-      </c>
+      <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>24</v>
       </c>
-      <c r="B25" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.65271179227895626</v>
-      </c>
+      <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>25</v>
       </c>
-      <c r="B26" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.33756549901657518</v>
-      </c>
+      <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>26</v>
       </c>
-      <c r="B27" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.41197948133229745</v>
-      </c>
+      <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>27</v>
       </c>
-      <c r="B28" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.24027960657660152</v>
-      </c>
+      <c r="B28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2838,7 +2449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B6"/>
     </sheetView>
   </sheetViews>
@@ -2864,7 +2475,7 @@
       </c>
       <c r="B2" s="2">
         <f ca="1">RAND()</f>
-        <v>0.36248620165624978</v>
+        <v>0.40126917969798326</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2873,7 +2484,7 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RAND()</f>
-        <v>0.54318775729180524</v>
+        <v>5.3863403111502506E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2882,7 +2493,7 @@
       </c>
       <c r="B4" s="2">
         <f ca="1">RAND()</f>
-        <v>0.67984716398740719</v>
+        <v>0.77906914303828356</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2891,7 +2502,7 @@
       </c>
       <c r="B5" s="2">
         <f ca="1">RAND()</f>
-        <v>0.95098998671837376</v>
+        <v>0.10076298299967956</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2900,7 +2511,7 @@
       </c>
       <c r="B6" s="2">
         <f ca="1">RAND()</f>
-        <v>0.85722802216256311</v>
+        <v>6.312425413190248E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2914,7 +2525,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2931,9 +2542,7 @@
       <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -2942,10 +2551,7 @@
       <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4">
-        <f t="shared" ref="C2:C28" ca="1" si="0">RAND()</f>
-        <v>0.12081862309495572</v>
-      </c>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -2954,10 +2560,7 @@
       <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.16450836079434361</v>
-      </c>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -2966,10 +2569,7 @@
       <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.3529706987609853</v>
-      </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -2978,10 +2578,7 @@
       <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.85013197924923811</v>
-      </c>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -2990,10 +2587,7 @@
       <c r="B6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.45951348758051458</v>
-      </c>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -3002,10 +2596,7 @@
       <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.75228770249748933</v>
-      </c>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -3014,10 +2605,7 @@
       <c r="B8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.15522907343010306</v>
-      </c>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -3026,10 +2614,7 @@
       <c r="B9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.79486829113050383</v>
-      </c>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -3038,10 +2623,7 @@
       <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.46719325738173223</v>
-      </c>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -3050,10 +2632,7 @@
       <c r="B11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.51142893459850236</v>
-      </c>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -3062,10 +2641,7 @@
       <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.9489069700819917E-3</v>
-      </c>
+      <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -3074,10 +2650,7 @@
       <c r="B13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.35605190520105578</v>
-      </c>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -3086,10 +2659,7 @@
       <c r="B14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.75682068420976778</v>
-      </c>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -3098,10 +2668,7 @@
       <c r="B15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.9874610904784547E-2</v>
-      </c>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -3110,10 +2677,7 @@
       <c r="B16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.97824375969191479</v>
-      </c>
+      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -3122,10 +2686,7 @@
       <c r="B17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.86930918804338697</v>
-      </c>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -3134,10 +2695,7 @@
       <c r="B18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.6571437494340705</v>
-      </c>
+      <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
@@ -3146,10 +2704,7 @@
       <c r="B19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.77735907305611429</v>
-      </c>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
@@ -3158,10 +2713,7 @@
       <c r="B20" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.80881448533205014</v>
-      </c>
+      <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
@@ -3170,10 +2722,7 @@
       <c r="B21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.1096967938932103</v>
-      </c>
+      <c r="C21" s="4"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
@@ -3182,10 +2731,7 @@
       <c r="B22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.58865760862828975</v>
-      </c>
+      <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
@@ -3194,10 +2740,7 @@
       <c r="B23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.31476474585215164</v>
-      </c>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -3206,10 +2749,7 @@
       <c r="B24" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.1516208548701572</v>
-      </c>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -3218,10 +2758,7 @@
       <c r="B25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.40924921783468349</v>
-      </c>
+      <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -3230,10 +2767,7 @@
       <c r="B26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.12807940855880973</v>
-      </c>
+      <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -3242,10 +2776,7 @@
       <c r="B27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.14543227478655096</v>
-      </c>
+      <c r="C27" s="4"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -3254,10 +2785,7 @@
       <c r="B28" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.70642256591474228</v>
-      </c>
+      <c r="C28" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3270,7 +2798,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3287,9 +2815,7 @@
       <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3298,10 +2824,7 @@
       <c r="B2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="4">
-        <f t="shared" ref="C2:C26" ca="1" si="0">RAND()</f>
-        <v>0.77226982438692393</v>
-      </c>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -3310,10 +2833,7 @@
       <c r="B3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.67475394229645058</v>
-      </c>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -3322,10 +2842,7 @@
       <c r="B4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.27568515045306097</v>
-      </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -3334,10 +2851,7 @@
       <c r="B5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.30621530934708152</v>
-      </c>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -3346,10 +2860,7 @@
       <c r="B6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.12962924963948319</v>
-      </c>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -3358,10 +2869,7 @@
       <c r="B7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.73390427278341985</v>
-      </c>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -3370,10 +2878,7 @@
       <c r="B8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.82868139663915796</v>
-      </c>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -3382,10 +2887,7 @@
       <c r="B9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.57050663682026692</v>
-      </c>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -3394,10 +2896,7 @@
       <c r="B10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.36288286653941326</v>
-      </c>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -3406,10 +2905,7 @@
       <c r="B11" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.36818691995197139</v>
-      </c>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -3418,10 +2914,7 @@
       <c r="B12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.19678208687800314</v>
-      </c>
+      <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -3430,10 +2923,7 @@
       <c r="B13" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.85664366108635548</v>
-      </c>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -3442,10 +2932,7 @@
       <c r="B14" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.83799660393075193</v>
-      </c>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -3454,10 +2941,7 @@
       <c r="B15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.66339728680664367</v>
-      </c>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -3466,10 +2950,7 @@
       <c r="B16" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.92821369054064384</v>
-      </c>
+      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -3478,10 +2959,7 @@
       <c r="B17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.13811087979279435</v>
-      </c>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -3490,10 +2968,7 @@
       <c r="B18" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.74630018936363285</v>
-      </c>
+      <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
@@ -3502,10 +2977,7 @@
       <c r="B19" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.29973785038261402</v>
-      </c>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
@@ -3514,10 +2986,7 @@
       <c r="B20" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.7842274491654736</v>
-      </c>
+      <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
@@ -3526,10 +2995,7 @@
       <c r="B21" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.70015986052640122</v>
-      </c>
+      <c r="C21" s="4"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
@@ -3538,10 +3004,7 @@
       <c r="B22" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.26359375911602823</v>
-      </c>
+      <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
@@ -3550,10 +3013,7 @@
       <c r="B23" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.23280876368002723</v>
-      </c>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -3562,10 +3022,7 @@
       <c r="B24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.45803594219971766</v>
-      </c>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -3574,10 +3031,7 @@
       <c r="B25" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.93827489223301075</v>
-      </c>
+      <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -3586,10 +3040,7 @@
       <c r="B26" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.6248847077654176</v>
-      </c>
+      <c r="C26" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3602,7 +3053,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3619,9 +3070,7 @@
       <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3630,10 +3079,7 @@
       <c r="B2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="4">
-        <f t="shared" ref="C2:C18" ca="1" si="0">RAND()</f>
-        <v>0.79856469279598619</v>
-      </c>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -3642,10 +3088,7 @@
       <c r="B3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.7235847684925466</v>
-      </c>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -3654,10 +3097,7 @@
       <c r="B4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.18237548937360837</v>
-      </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -3666,10 +3106,7 @@
       <c r="B5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.70572273154090104</v>
-      </c>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -3678,10 +3115,7 @@
       <c r="B6" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.80746164323463587</v>
-      </c>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -3690,10 +3124,7 @@
       <c r="B7" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.10760014454805655</v>
-      </c>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -3702,10 +3133,7 @@
       <c r="B8" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.41883102171394715</v>
-      </c>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -3714,10 +3142,7 @@
       <c r="B9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.80378238574358918</v>
-      </c>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -3726,10 +3151,7 @@
       <c r="B10" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.64143101306831019</v>
-      </c>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -3738,10 +3160,7 @@
       <c r="B11" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.29844337282091093</v>
-      </c>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -3750,10 +3169,7 @@
       <c r="B12" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.24300674038508685</v>
-      </c>
+      <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -3762,10 +3178,7 @@
       <c r="B13" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.27296521279402475</v>
-      </c>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -3774,10 +3187,7 @@
       <c r="B14" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.31551658733959287</v>
-      </c>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -3786,10 +3196,7 @@
       <c r="B15" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.8474376806922661</v>
-      </c>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -3798,10 +3205,7 @@
       <c r="B16" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.68361326337141193</v>
-      </c>
+      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -3810,10 +3214,7 @@
       <c r="B17" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.45045840109899571</v>
-      </c>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -3822,10 +3223,7 @@
       <c r="B18" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.6127235550741199E-2</v>
-      </c>
+      <c r="C18" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3838,7 +3236,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3860,9 +3258,7 @@
       <c r="C1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -3874,10 +3270,7 @@
       <c r="C2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="6">
-        <f t="shared" ref="D2:D43" ca="1" si="0">RAND()</f>
-        <v>8.0147519264704647E-2</v>
-      </c>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -3889,10 +3282,7 @@
       <c r="C3" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D3" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.91569901290764655</v>
-      </c>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -3904,10 +3294,7 @@
       <c r="C4" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.49755680679415382</v>
-      </c>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -3919,10 +3306,7 @@
       <c r="C5" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.53167072576886865</v>
-      </c>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -3934,10 +3318,7 @@
       <c r="C6" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D6" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.22443188990407081</v>
-      </c>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -3949,10 +3330,7 @@
       <c r="C7" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D7" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.9842486931288761E-2</v>
-      </c>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -3964,10 +3342,7 @@
       <c r="C8" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D8" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.56702862013204136</v>
-      </c>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -3979,10 +3354,7 @@
       <c r="C9" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.97427460344852679</v>
-      </c>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -3994,10 +3366,7 @@
       <c r="C10" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.73615103167956497</v>
-      </c>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -4009,10 +3378,7 @@
       <c r="C11" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D11" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.23919804090899899</v>
-      </c>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -4024,10 +3390,7 @@
       <c r="C12" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D12" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.37627136832975039</v>
-      </c>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -4039,10 +3402,7 @@
       <c r="C13" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D13" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.3935147298651547E-3</v>
-      </c>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -4054,10 +3414,7 @@
       <c r="C14" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="D14" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.10588094285458571</v>
-      </c>
+      <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
@@ -4069,10 +3426,7 @@
       <c r="C15" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D15" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.55416112257745087</v>
-      </c>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
@@ -4084,10 +3438,7 @@
       <c r="C16" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="D16" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.70581010310464953</v>
-      </c>
+      <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -4099,10 +3450,7 @@
       <c r="C17" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="D17" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.16864431467702645</v>
-      </c>
+      <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
@@ -4114,10 +3462,7 @@
       <c r="C18" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="D18" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.453555864396879</v>
-      </c>
+      <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
@@ -4129,10 +3474,7 @@
       <c r="C19" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D19" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.65500902777586245</v>
-      </c>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
@@ -4144,10 +3486,7 @@
       <c r="C20" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="D20" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.72243037786299247</v>
-      </c>
+      <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
@@ -4159,10 +3498,7 @@
       <c r="C21" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.45383352471849348</v>
-      </c>
+      <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
@@ -4174,10 +3510,7 @@
       <c r="C22" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D22" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.22035195738514257</v>
-      </c>
+      <c r="D22" s="6"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
@@ -4189,10 +3522,7 @@
       <c r="C23" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D23" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.32357285032479799</v>
-      </c>
+      <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
@@ -4204,10 +3534,7 @@
       <c r="C24" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D24" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.18313718577820104</v>
-      </c>
+      <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
@@ -4219,10 +3546,7 @@
       <c r="C25" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="D25" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.55990686531065015</v>
-      </c>
+      <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
@@ -4234,10 +3558,7 @@
       <c r="C26" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D26" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.82806063990487755</v>
-      </c>
+      <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
@@ -4249,10 +3570,7 @@
       <c r="C27" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="D27" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.52009750181189851</v>
-      </c>
+      <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
@@ -4264,10 +3582,7 @@
       <c r="C28" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="D28" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.48690986006134229</v>
-      </c>
+      <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
@@ -4279,10 +3594,7 @@
       <c r="C29" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="D29" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.30962347933176704</v>
-      </c>
+      <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
@@ -4294,10 +3606,7 @@
       <c r="C30" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="D30" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.98649722747867008</v>
-      </c>
+      <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
@@ -4309,10 +3618,7 @@
       <c r="C31" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D31" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.29149133628824475</v>
-      </c>
+      <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
@@ -4324,10 +3630,7 @@
       <c r="C32" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="D32" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.38552030076813348</v>
-      </c>
+      <c r="D32" s="6"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
@@ -4339,10 +3642,7 @@
       <c r="C33" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="D33" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.24447305482737747</v>
-      </c>
+      <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
@@ -4354,10 +3654,7 @@
       <c r="C34" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="D34" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.46235923335595919</v>
-      </c>
+      <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
@@ -4369,10 +3666,7 @@
       <c r="C35" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="D35" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.86542881547921857</v>
-      </c>
+      <c r="D35" s="6"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
@@ -4384,10 +3678,7 @@
       <c r="C36" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="D36" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.43133150539403065</v>
-      </c>
+      <c r="D36" s="6"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
@@ -4399,10 +3690,7 @@
       <c r="C37" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D37" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.31161147966128055</v>
-      </c>
+      <c r="D37" s="6"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
@@ -4414,10 +3702,7 @@
       <c r="C38" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="D38" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.48319161105044484</v>
-      </c>
+      <c r="D38" s="6"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
@@ -4429,10 +3714,7 @@
       <c r="C39" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="D39" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.13561044516723131</v>
-      </c>
+      <c r="D39" s="6"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
@@ -4444,10 +3726,7 @@
       <c r="C40" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D40" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.58295590614305581</v>
-      </c>
+      <c r="D40" s="6"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
@@ -4459,10 +3738,7 @@
       <c r="C41" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="D41" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.23926628118462012</v>
-      </c>
+      <c r="D41" s="6"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
@@ -4474,10 +3750,7 @@
       <c r="C42" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="D42" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.62673847385073811</v>
-      </c>
+      <c r="D42" s="6"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
@@ -4489,10 +3762,7 @@
       <c r="C43" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="D43" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.6772078275660568</v>
-      </c>
+      <c r="D43" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4505,7 +3775,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4527,9 +3797,7 @@
       <c r="D1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
@@ -4544,10 +3812,7 @@
       <c r="D2" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E2" s="2">
-        <f t="shared" ref="E2:E16" ca="1" si="0">RAND()</f>
-        <v>0.54614731436952468</v>
-      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -4562,10 +3827,7 @@
       <c r="D3" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E3" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.33803655308379499</v>
-      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
@@ -4580,10 +3842,7 @@
       <c r="D4" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.3587341039354871</v>
-      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
@@ -4598,10 +3857,7 @@
       <c r="D5" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.28668801974961367</v>
-      </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
@@ -4616,10 +3872,7 @@
       <c r="D6" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.28429787736295509</v>
-      </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -4634,10 +3887,7 @@
       <c r="D7" s="8">
         <v>5.5</v>
       </c>
-      <c r="E7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.61940082638873961</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
@@ -4652,10 +3902,7 @@
       <c r="D8" s="8">
         <v>5.5</v>
       </c>
-      <c r="E8" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.73658297596761801</v>
-      </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
@@ -4670,10 +3917,7 @@
       <c r="D9" s="8">
         <v>5.5</v>
       </c>
-      <c r="E9" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.84257621602912869</v>
-      </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
@@ -4688,10 +3932,7 @@
       <c r="D10" s="8">
         <v>5.5</v>
       </c>
-      <c r="E10" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.68814535131457066</v>
-      </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
@@ -4706,10 +3947,7 @@
       <c r="D11" s="8">
         <v>5.5</v>
       </c>
-      <c r="E11" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.63451499526329835</v>
-      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
@@ -4724,10 +3962,7 @@
       <c r="D12" s="8">
         <v>6.4</v>
       </c>
-      <c r="E12" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.41466282225764561</v>
-      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -4742,10 +3977,7 @@
       <c r="D13" s="8">
         <v>6.4</v>
       </c>
-      <c r="E13" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.69657282580336088</v>
-      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
@@ -4760,10 +3992,7 @@
       <c r="D14" s="8">
         <v>6.4</v>
       </c>
-      <c r="E14" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.78277521378257597</v>
-      </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -4778,10 +4007,7 @@
       <c r="D15" s="8">
         <v>6.4</v>
       </c>
-      <c r="E15" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.58143021180533794</v>
-      </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
@@ -4796,10 +4022,7 @@
       <c r="D16" s="8">
         <v>6.4</v>
       </c>
-      <c r="E16" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.4291915888739869</v>
-      </c>
+      <c r="E16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4812,7 +4035,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4834,9 +4057,7 @@
       <c r="D1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
@@ -4851,10 +4072,7 @@
       <c r="D2" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E2" s="2">
-        <f t="shared" ref="E2:E16" ca="1" si="0">RAND()</f>
-        <v>0.48693294060494086</v>
-      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -4869,10 +4087,7 @@
       <c r="D3" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E3" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.88330658743485979</v>
-      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
@@ -4887,10 +4102,7 @@
       <c r="D4" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.72095854487992328</v>
-      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
@@ -4905,10 +4117,7 @@
       <c r="D5" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.93239556104052967</v>
-      </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
@@ -4923,10 +4132,7 @@
       <c r="D6" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.75650786521673774</v>
-      </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -4941,10 +4147,7 @@
       <c r="D7" s="8">
         <v>5.5</v>
       </c>
-      <c r="E7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.49871771877622262</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
@@ -4959,10 +4162,7 @@
       <c r="D8" s="8">
         <v>5.5</v>
       </c>
-      <c r="E8" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.5654314487352714</v>
-      </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
@@ -4977,10 +4177,7 @@
       <c r="D9" s="8">
         <v>5.5</v>
       </c>
-      <c r="E9" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.75007170976488435</v>
-      </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
@@ -4995,10 +4192,7 @@
       <c r="D10" s="8">
         <v>5.5</v>
       </c>
-      <c r="E10" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.14350187114798629</v>
-      </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
@@ -5013,10 +4207,7 @@
       <c r="D11" s="8">
         <v>5.5</v>
       </c>
-      <c r="E11" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.16278025899129656</v>
-      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
@@ -5031,10 +4222,7 @@
       <c r="D12" s="8">
         <v>6.4</v>
       </c>
-      <c r="E12" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.86955106327075948</v>
-      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -5049,10 +4237,7 @@
       <c r="D13" s="8">
         <v>6.4</v>
       </c>
-      <c r="E13" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.90371812151442898</v>
-      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
@@ -5067,10 +4252,7 @@
       <c r="D14" s="8">
         <v>6.4</v>
       </c>
-      <c r="E14" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.74005310195215579</v>
-      </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -5085,10 +4267,7 @@
       <c r="D15" s="8">
         <v>6.4</v>
       </c>
-      <c r="E15" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.40367521330996436</v>
-      </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
@@ -5103,10 +4282,7 @@
       <c r="D16" s="8">
         <v>6.4</v>
       </c>
-      <c r="E16" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.68995023011270307</v>
-      </c>
+      <c r="E16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -5119,7 +4295,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5141,9 +4317,7 @@
       <c r="D1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
@@ -5158,10 +4332,7 @@
       <c r="D2" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E2" s="2">
-        <f t="shared" ref="E2:E16" ca="1" si="0">RAND()</f>
-        <v>0.27432203574036551</v>
-      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -5176,10 +4347,7 @@
       <c r="D3" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E3" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.79508839308510249</v>
-      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
@@ -5194,10 +4362,7 @@
       <c r="D4" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.21806237968901121</v>
-      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
@@ -5212,10 +4377,7 @@
       <c r="D5" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.59163131886622022</v>
-      </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
@@ -5230,10 +4392,7 @@
       <c r="D6" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.23697997927378189</v>
-      </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -5248,10 +4407,7 @@
       <c r="D7" s="8">
         <v>5.5</v>
       </c>
-      <c r="E7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.39891594544214282</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
@@ -5266,10 +4422,7 @@
       <c r="D8" s="8">
         <v>5.5</v>
       </c>
-      <c r="E8" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.53352062596592043</v>
-      </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
@@ -5284,10 +4437,7 @@
       <c r="D9" s="8">
         <v>5.5</v>
       </c>
-      <c r="E9" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.7386325829493583</v>
-      </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
@@ -5302,10 +4452,7 @@
       <c r="D10" s="8">
         <v>5.5</v>
       </c>
-      <c r="E10" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.25458035561871706</v>
-      </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
@@ -5320,10 +4467,7 @@
       <c r="D11" s="8">
         <v>5.5</v>
       </c>
-      <c r="E11" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.8288249737817286E-2</v>
-      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
@@ -5338,10 +4482,7 @@
       <c r="D12" s="8">
         <v>6.4</v>
       </c>
-      <c r="E12" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.64057115724445035</v>
-      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -5356,10 +4497,7 @@
       <c r="D13" s="8">
         <v>6.4</v>
       </c>
-      <c r="E13" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.45003278333461816</v>
-      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
@@ -5374,10 +4512,7 @@
       <c r="D14" s="8">
         <v>6.4</v>
       </c>
-      <c r="E14" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.81701367239285128</v>
-      </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -5392,10 +4527,7 @@
       <c r="D15" s="8">
         <v>6.4</v>
       </c>
-      <c r="E15" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.21155322332381643</v>
-      </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
@@ -5410,10 +4542,7 @@
       <c r="D16" s="8">
         <v>6.4</v>
       </c>
-      <c r="E16" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.79654270095315782</v>
-      </c>
+      <c r="E16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -5426,7 +4555,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5439,81 +4568,55 @@
       <c r="A1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>5.7</v>
       </c>
-      <c r="B2" s="2">
-        <f t="shared" ref="B2:B9" ca="1" si="0">RAND()</f>
-        <v>0.92718379323394284</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>5.7</v>
       </c>
-      <c r="B3" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.32575798073260476</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>6.6</v>
       </c>
-      <c r="B4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.57450470485529981</v>
-      </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>6.6</v>
       </c>
-      <c r="B5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.31345017501578543</v>
-      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>6.6</v>
       </c>
-      <c r="B6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.62301487514590814</v>
-      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6.6</v>
       </c>
-      <c r="B7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.59335253331055648</v>
-      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7.5</v>
       </c>
-      <c r="B8" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.95470660712360611</v>
-      </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7.5</v>
       </c>
-      <c r="B9" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.9998176849693783E-3</v>
-      </c>
+      <c r="B9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>